<commit_message>
MTR-2464 updated TC-15288 TC-16647 added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/VOLHO3.xlsx
+++ b/src/test/resources/testdata/VOLHO3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9396A69E-ED85-4D5D-946E-3EB6667BD82C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC3F7BC-5C7E-4BDB-A28C-A7B6E04D1541}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="19416" windowHeight="10416" xr2:uid="{CD3A54CB-C005-0E4A-932C-421D6A132F4C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
   <si>
     <t>FirstName</t>
   </si>
@@ -123,19 +123,16 @@
     <t>Economy</t>
   </si>
   <si>
-    <t>Standard</t>
+    <t>12012023</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
   <si>
     <t>6268 Dolostone Dr</t>
   </si>
   <si>
     <t>33811</t>
-  </si>
-  <si>
-    <t>11012023</t>
-  </si>
-  <si>
-    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -508,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D793F7-630D-9741-BAE5-9B86014DDE1E}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -601,7 +598,7 @@
         <v>33837</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -610,7 +607,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>25</v>
@@ -625,7 +622,7 @@
         <v>24</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>29</v>
@@ -645,13 +642,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
@@ -660,7 +657,7 @@
         <v>16</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>26</v>
@@ -675,13 +672,13 @@
         <v>24</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.4">
@@ -701,7 +698,7 @@
         <v>33837</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -710,7 +707,7 @@
         <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>25</v>
@@ -725,7 +722,7 @@
         <v>24</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>29</v>
@@ -745,13 +742,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -760,7 +757,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>26</v>
@@ -775,13 +772,13 @@
         <v>24</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="21" x14ac:dyDescent="0.4">
@@ -801,7 +798,7 @@
         <v>33837</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
@@ -810,7 +807,7 @@
         <v>16</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>25</v>
@@ -825,7 +822,7 @@
         <v>24</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>29</v>
@@ -834,7 +831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -845,13 +842,13 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>14</v>
@@ -860,7 +857,7 @@
         <v>16</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>26</v>
@@ -875,13 +872,13 @@
         <v>24</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.4">
@@ -901,7 +898,7 @@
         <v>33837</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
@@ -910,7 +907,7 @@
         <v>16</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>25</v>
@@ -925,7 +922,7 @@
         <v>24</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>29</v>
@@ -935,78 +932,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>